<commit_message>
SerializationReader works but is much less efficient than needed.
</commit_message>
<xml_diff>
--- a/DocxDocument.ReadWrite.Test/SampleDocs/PageSizes.xlsx
+++ b/DocxDocument.ReadWrite.Test/SampleDocs/PageSizes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS\Projects\DocxDocument\DocxDocument.ReadWrite.Test\SampleDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2248F3D5-3A37-4169-8476-90EA1A7DFCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF9669E-AB0A-45BA-8308-C7FDAAC15287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2B816884-F8C3-4D8C-BFB6-373AFCDC8165}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="143">
   <si>
     <t>Letter</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>};</t>
+  </si>
+  <si>
+    <t>EnvelopeChou4</t>
   </si>
 </sst>
 </file>
@@ -2415,8 +2418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF113EA-22A7-4763-B694-7A143D056942}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4059,7 +4062,7 @@
         <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="C46" t="s">
         <v>58</v>
@@ -4087,7 +4090,7 @@
       <c r="J46" s="3"/>
       <c r="K46" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  EnvelopeChou3 = 74,</v>
+        <v xml:space="preserve">  EnvelopeChou4 = 74,</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>